<commit_message>
implemented the paralel option
</commit_message>
<xml_diff>
--- a/src/test/resources/com/prestashop/test-data/Products.xlsx
+++ b/src/test/resources/com/prestashop/test-data/Products.xlsx
@@ -1,22 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cybertekschool/JavaPrgs/acceptance-tests/src/test/resources/com/prestashop/test-data/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{0BFBB9C9-C6EA-E342-8DFC-9F2C87E8047E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34"/>
+  <xr:revisionPtr documentId="13_ncr:801_{FEE8F5BF-739D-416B-8A4A-7DAB3B93F968}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36"/>
   <bookViews>
-    <workbookView activeTab="1" tabRatio="500" windowHeight="20980" windowWidth="40960" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="460"/>
+    <workbookView tabRatio="500" windowHeight="7815" windowWidth="16635" xWindow="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
     <sheet name="sort" r:id="rId2" sheetId="2"/>
   </sheets>
-  <calcPr calcId="150000"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:C8"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -29,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="39">
   <si>
     <t>Execute</t>
   </si>
@@ -469,17 +465,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="157">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0" zoomScale="256">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.83203125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.8125" collapsed="true"/>
     <col min="3" max="6" customWidth="true" width="16.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,9 +498,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
@@ -522,10 +518,10 @@
         <v>24</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -548,7 +544,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -571,7 +567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -604,17 +600,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{333419CA-489B-534C-9571-ABC48E4CE77F}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScale="256">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="A5" workbookViewId="0" zoomScale="256">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
     <col min="2" max="2" bestFit="true" customWidth="true" width="37.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="36.1640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="36.1875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -631,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -648,7 +644,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -665,7 +661,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -682,7 +678,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -699,7 +695,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -716,7 +712,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -733,7 +729,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
         <v>3</v>
       </c>

</xml_diff>